<commit_message>
owe ir review added
</commit_message>
<xml_diff>
--- a/PUwisedetails.xlsx
+++ b/PUwisedetails.xlsx
@@ -615,17 +615,17 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>JUN' 21</t>
+          <t>OCT' 21</t>
         </is>
       </c>
       <c r="E3" s="8" t="inlineStr">
         <is>
-          <t>JUN' 22</t>
+          <t>OCT' 22</t>
         </is>
       </c>
       <c r="F3" s="8" t="inlineStr">
         <is>
-          <t>JUN' 22</t>
+          <t>OCT' 22</t>
         </is>
       </c>
       <c r="G3" s="8" t="inlineStr">
@@ -667,13 +667,13 @@
         <v>2555.5</v>
       </c>
       <c r="D4" t="n">
-        <v>643.91</v>
+        <v>1507.04</v>
       </c>
       <c r="E4" t="n">
-        <v>665.24</v>
+        <v>1535.17</v>
       </c>
       <c r="F4" t="n">
-        <v>662.58</v>
+        <v>1528.7</v>
       </c>
       <c r="G4">
         <f>F4-E4</f>
@@ -709,13 +709,13 @@
         <v>231.76</v>
       </c>
       <c r="D5" t="n">
-        <v>53.42</v>
+        <v>131.63</v>
       </c>
       <c r="E5" t="n">
-        <v>60.26</v>
+        <v>139.05</v>
       </c>
       <c r="F5" t="n">
-        <v>84.38</v>
+        <v>169.97</v>
       </c>
       <c r="G5">
         <f>F5-E5</f>
@@ -751,13 +751,13 @@
         <v>4.27</v>
       </c>
       <c r="D6" t="n">
-        <v>0.43</v>
+        <v>0.99</v>
       </c>
       <c r="E6" t="n">
-        <v>1.11</v>
+        <v>2.56</v>
       </c>
       <c r="F6" t="n">
-        <v>3.32</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="G6">
         <f>F6-E6</f>
@@ -793,13 +793,13 @@
         <v>8.720000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>1.38</v>
+        <v>4.04</v>
       </c>
       <c r="E7" t="n">
-        <v>2.27</v>
+        <v>5.23</v>
       </c>
       <c r="F7" t="n">
-        <v>2.53</v>
+        <v>5.5</v>
       </c>
       <c r="G7">
         <f>F7-E7</f>
@@ -832,16 +832,16 @@
         <v>350.79</v>
       </c>
       <c r="C8" t="n">
-        <v>298.86</v>
+        <v>305.42</v>
       </c>
       <c r="D8" t="n">
-        <v>79.69</v>
+        <v>209.56</v>
       </c>
       <c r="E8" t="n">
-        <v>77.7</v>
+        <v>173.34</v>
       </c>
       <c r="F8" t="n">
-        <v>102.77</v>
+        <v>230.28</v>
       </c>
       <c r="G8">
         <f>F8-E8</f>

</xml_diff>